<commit_message>
Corregida Grid, reinciado el PCB
Crroegido grid a 25 mil, reconectado el layout, se cambiaron ubicación de algunos elementos dentro de la sabana . se retiraron las resistencias de 0 ohm no necesarias en la I/O, se cambio bonina por resistencia de p ohm en diagrama reset se agregó resistencias pull up a I2C, , se reitaron resistencias pull up no necesarias en la conexion de la Micro SD. Se organizaron las fuentes de todo el circuito, 3.3V Alimentación 3V3 punto de conexion ESP  y 3.3VP punto de conexion Lora.
</commit_message>
<xml_diff>
--- a/Info/Comparativos.xlsx
+++ b/Info/Comparativos.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poved\OneDrive - Blackstone\Maestria\Semestre I\Fabricacion SE\Microcontrolador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poved\OneDrive - Blackstone\Maestria\Semestre I\Fabricacion SE\SE_Datalog\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Descripcion</t>
   </si>
@@ -433,6 +434,48 @@
   <si>
     <t>SX1272/73 - 860 MHz to 1020 MHz Low Power Long Range Transceiver
 SEMTECH</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical </t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>Recomendado</t>
+  </si>
+  <si>
+    <t>Absoluta</t>
+  </si>
+  <si>
+    <t>I mA</t>
+  </si>
+  <si>
+    <t>Absoluto</t>
+  </si>
+  <si>
+    <t>Lora</t>
+  </si>
+  <si>
+    <t>ImA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a 3,3 V </t>
+  </si>
+  <si>
+    <t>pagina 13</t>
+  </si>
+  <si>
+    <t>transmitiendo</t>
   </si>
 </sst>
 </file>
@@ -472,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +525,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -568,6 +623,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -585,6 +662,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>103252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>735213</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>153223</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="2198752"/>
+          <a:ext cx="6307338" cy="2907471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1037,4 +1157,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D4" s="23">
+        <v>-0.3</v>
+      </c>
+      <c r="E4" s="23">
+        <v>500</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="H4" s="24">
+        <v>-0.5</v>
+      </c>
+      <c r="I4" s="24">
+        <v>20</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="23">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24">
+        <v>120</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="D6" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24">
+        <v>1100</v>
+      </c>
+      <c r="G6" s="24">
+        <v>3.7</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3.9</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I7" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>